<commit_message>
Support Sheet rename in mainbook model.
</commit_message>
<xml_diff>
--- a/test1/mwb.xlsx
+++ b/test1/mwb.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>__workbook__</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,10 @@
   </si>
   <si>
     <t>wb2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作表4-&gt;工作表4改</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -156,8 +160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -171,13 +177,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -610,6 +618,11 @@
     <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>